<commit_message>
Add reasoning to checklist
</commit_message>
<xml_diff>
--- a/Exc2/Checklist.xlsx
+++ b/Exc2/Checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita.Chertov\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita.Chertov\IdeaProjects\architecture-sprint-7\Exc2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB73C377-9E34-4FE7-8678-803A6F9BDBBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1D3B77-5C10-4DFD-8270-D2E9589827C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2796" yWindow="0" windowWidth="27876" windowHeight="12996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="86">
   <si>
     <t>№</t>
   </si>
@@ -255,6 +255,30 @@
   </si>
   <si>
     <t>3. Облачная инфраструктура</t>
+  </si>
+  <si>
+    <t>Обоснование включения раздела в список</t>
+  </si>
+  <si>
+    <t>Руководство обеспокоено утечкой данных у конкурентов. Вопросам доступа к информации внутри систем нужно уделить достаточное внимание.</t>
+  </si>
+  <si>
+    <t>Раздел "безопасть данных" также поднимает вопросы защиты данных от несанкионированного доступа, и затрагивает тему соответствия требованиям законодательства, которой заинтересовано руководство компании.</t>
+  </si>
+  <si>
+    <t>Компания располагает собственными серверами, так что данный раздел для неё актуален.</t>
+  </si>
+  <si>
+    <t>Раздел включен в виду использования облачной инфраструктуры.</t>
+  </si>
+  <si>
+    <t>Компания имеет определенный IT-ландшафт и заботится вопросами его безопасноти, поэтому вопросы защиты имеющейся инфраструктуры важны.</t>
+  </si>
+  <si>
+    <t>Общие вопросы безопасности доступа.</t>
+  </si>
+  <si>
+    <t>Реагирование на инциденты заявлено как одна из потребностей бизнеса.</t>
   </si>
 </sst>
 </file>
@@ -300,7 +324,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -360,11 +384,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -406,6 +448,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,22 +685,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:F70"/>
+  <dimension ref="B3:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.44140625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" ht="27" customHeight="1">
+    <row r="3" spans="3:9" ht="27" customHeight="1">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,16 +714,24 @@
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="3:6" ht="30.75" customHeight="1">
+      <c r="G3" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" ht="30.75" customHeight="1">
       <c r="C4" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="3:6" ht="83.45" customHeight="1">
+      <c r="G4" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="3:9" ht="83.4" customHeight="1">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -682,8 +742,9 @@
         <v>64</v>
       </c>
       <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="3:6" ht="61.5" customHeight="1">
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="3:9" ht="61.5" customHeight="1">
       <c r="C6" s="2">
         <v>2</v>
       </c>
@@ -695,7 +756,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="3:6" ht="80.25" customHeight="1">
+    <row r="7" spans="3:9" ht="80.25" customHeight="1">
       <c r="C7" s="2">
         <v>3</v>
       </c>
@@ -707,7 +768,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="3:6" ht="77.25" customHeight="1">
+    <row r="8" spans="3:9" ht="77.25" customHeight="1">
       <c r="C8" s="2">
         <v>4</v>
       </c>
@@ -719,7 +780,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="3:6" ht="87.75" customHeight="1">
+    <row r="9" spans="3:9" ht="87.75" customHeight="1">
       <c r="C9" s="2">
         <v>5</v>
       </c>
@@ -731,7 +792,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="3:6" ht="69" customHeight="1">
+    <row r="10" spans="3:9" ht="69" customHeight="1">
       <c r="C10" s="2">
         <v>6</v>
       </c>
@@ -743,7 +804,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="3:6" ht="82.5" customHeight="1">
+    <row r="11" spans="3:9" ht="82.5" customHeight="1">
       <c r="C11" s="2">
         <v>7</v>
       </c>
@@ -755,7 +816,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="3:6" ht="62.25" customHeight="1">
+    <row r="12" spans="3:9" ht="62.25" customHeight="1">
       <c r="C12" s="2">
         <v>8</v>
       </c>
@@ -767,7 +828,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="3:6" ht="55.5" customHeight="1">
+    <row r="13" spans="3:9" ht="55.5" customHeight="1">
       <c r="C13" s="2">
         <v>9</v>
       </c>
@@ -779,7 +840,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="3:6" ht="62.45" customHeight="1">
+    <row r="14" spans="3:9" ht="62.4" customHeight="1">
       <c r="C14" s="2">
         <v>10</v>
       </c>
@@ -791,7 +852,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="3:6" ht="62.45" customHeight="1">
+    <row r="15" spans="3:9" ht="62.4" customHeight="1">
       <c r="C15" s="2">
         <v>11</v>
       </c>
@@ -803,7 +864,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="3:6" ht="68.25" customHeight="1">
+    <row r="16" spans="3:9" ht="68.25" customHeight="1">
       <c r="C16" s="2">
         <v>12</v>
       </c>
@@ -815,7 +876,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="3:6" ht="52.9" customHeight="1">
+    <row r="17" spans="3:7" ht="52.95" customHeight="1">
       <c r="C17" s="2">
         <v>13</v>
       </c>
@@ -827,7 +888,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="3:6" ht="60.75" customHeight="1">
+    <row r="18" spans="3:7" ht="60.75" customHeight="1">
       <c r="C18" s="2">
         <v>14</v>
       </c>
@@ -839,15 +900,18 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="3:6" ht="36.75" customHeight="1">
+    <row r="19" spans="3:7" ht="36.75" customHeight="1">
       <c r="C19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
-    </row>
-    <row r="20" spans="3:6" ht="75.75" customHeight="1">
+      <c r="G19" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" ht="75.75" customHeight="1">
       <c r="C20" s="2">
         <v>1</v>
       </c>
@@ -858,8 +922,9 @@
         <v>66</v>
       </c>
       <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="3:6" ht="63.75" customHeight="1">
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="3:7" ht="63.75" customHeight="1">
       <c r="C21" s="2">
         <v>2</v>
       </c>
@@ -870,8 +935,9 @@
         <v>64</v>
       </c>
       <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="3:6" ht="54" customHeight="1">
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="3:7" ht="54" customHeight="1">
       <c r="C22" s="2">
         <v>3</v>
       </c>
@@ -883,7 +949,7 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="3:6" ht="82.5" customHeight="1">
+    <row r="23" spans="3:7" ht="82.5" customHeight="1">
       <c r="C23" s="2">
         <v>4</v>
       </c>
@@ -897,7 +963,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="3:6" ht="64.5" customHeight="1">
+    <row r="24" spans="3:7" ht="64.5" customHeight="1">
       <c r="C24" s="2">
         <v>5</v>
       </c>
@@ -909,7 +975,7 @@
       </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="3:6" ht="56.25" customHeight="1">
+    <row r="25" spans="3:7" ht="56.25" customHeight="1">
       <c r="C25" s="2">
         <v>6</v>
       </c>
@@ -921,7 +987,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="3:6" ht="125.25" customHeight="1">
+    <row r="26" spans="3:7" ht="125.25" customHeight="1">
       <c r="C26" s="2">
         <v>7</v>
       </c>
@@ -935,7 +1001,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="3:6" ht="90" customHeight="1">
+    <row r="27" spans="3:7" ht="90" customHeight="1">
       <c r="C27" s="2">
         <v>8</v>
       </c>
@@ -949,7 +1015,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="3:6" ht="55.5" customHeight="1">
+    <row r="28" spans="3:7" ht="55.5" customHeight="1">
       <c r="C28" s="2">
         <v>9</v>
       </c>
@@ -961,7 +1027,7 @@
       </c>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="3:6" ht="51.75" customHeight="1">
+    <row r="29" spans="3:7" ht="51.75" customHeight="1">
       <c r="C29" s="2">
         <v>10</v>
       </c>
@@ -973,7 +1039,7 @@
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="3:6" ht="53.25" customHeight="1">
+    <row r="30" spans="3:7" ht="53.25" customHeight="1">
       <c r="C30" s="2">
         <v>11</v>
       </c>
@@ -985,7 +1051,7 @@
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="3:6" ht="52.5" customHeight="1">
+    <row r="31" spans="3:7" ht="52.5" customHeight="1">
       <c r="C31" s="2">
         <v>12</v>
       </c>
@@ -997,7 +1063,7 @@
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="3:6" ht="51" customHeight="1">
+    <row r="32" spans="3:7" ht="51" customHeight="1">
       <c r="C32" s="2">
         <v>13</v>
       </c>
@@ -1009,7 +1075,7 @@
       </c>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="3:6" ht="48.75" customHeight="1">
+    <row r="33" spans="3:7" ht="48.75" customHeight="1">
       <c r="C33" s="2">
         <v>14</v>
       </c>
@@ -1021,15 +1087,18 @@
       </c>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="3:6" ht="29.25" customHeight="1">
+    <row r="34" spans="3:7" ht="29.25" customHeight="1">
       <c r="C34" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
-    </row>
-    <row r="35" spans="3:6" ht="69" customHeight="1">
+      <c r="G34" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" ht="69" customHeight="1">
       <c r="C35" s="2">
         <v>1</v>
       </c>
@@ -1040,8 +1109,9 @@
         <v>65</v>
       </c>
       <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="3:6" ht="90.75" customHeight="1">
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="3:7" ht="90.75" customHeight="1">
       <c r="C36" s="2">
         <v>2</v>
       </c>
@@ -1053,7 +1123,7 @@
       </c>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="3:6" ht="80.25" customHeight="1">
+    <row r="37" spans="3:7" ht="80.25" customHeight="1">
       <c r="C37" s="2">
         <v>3</v>
       </c>
@@ -1065,7 +1135,7 @@
       </c>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="3:6" ht="70.5" customHeight="1">
+    <row r="38" spans="3:7" ht="70.5" customHeight="1">
       <c r="C38" s="2">
         <v>4</v>
       </c>
@@ -1077,7 +1147,7 @@
       </c>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="3:6" ht="80.25" customHeight="1">
+    <row r="39" spans="3:7" ht="80.25" customHeight="1">
       <c r="C39" s="2">
         <v>5</v>
       </c>
@@ -1089,7 +1159,7 @@
       </c>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="3:6" ht="82.5" customHeight="1">
+    <row r="40" spans="3:7" ht="82.5" customHeight="1">
       <c r="C40" s="2">
         <v>6</v>
       </c>
@@ -1101,7 +1171,7 @@
       </c>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="3:6" ht="81" customHeight="1">
+    <row r="41" spans="3:7" ht="81" customHeight="1">
       <c r="C41" s="2">
         <v>7</v>
       </c>
@@ -1113,7 +1183,7 @@
       </c>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="3:6" ht="78.75" customHeight="1">
+    <row r="42" spans="3:7" ht="78.75" customHeight="1">
       <c r="C42" s="2">
         <v>8</v>
       </c>
@@ -1125,7 +1195,7 @@
       </c>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="3:6" ht="93.75" customHeight="1">
+    <row r="43" spans="3:7" ht="93.75" customHeight="1">
       <c r="C43" s="2">
         <v>9</v>
       </c>
@@ -1137,7 +1207,7 @@
       </c>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="3:6" ht="63.75" customHeight="1">
+    <row r="44" spans="3:7" ht="63.75" customHeight="1">
       <c r="C44" s="2">
         <v>10</v>
       </c>
@@ -1149,7 +1219,7 @@
       </c>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="3:6" ht="53.25" customHeight="1">
+    <row r="45" spans="3:7" ht="53.25" customHeight="1">
       <c r="C45" s="2">
         <v>11</v>
       </c>
@@ -1163,7 +1233,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="3:6" ht="54.75" customHeight="1">
+    <row r="46" spans="3:7" ht="54.75" customHeight="1">
       <c r="C46" s="2">
         <v>12</v>
       </c>
@@ -1175,15 +1245,18 @@
       </c>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="3:6" ht="24.75" customHeight="1">
+    <row r="47" spans="3:7" ht="24.75" customHeight="1">
       <c r="C47" s="15" t="s">
         <v>47</v>
       </c>
       <c r="D47" s="15"/>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
-    </row>
-    <row r="48" spans="3:6" ht="82.5" customHeight="1">
+      <c r="G47" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" ht="82.5" customHeight="1">
       <c r="C48" s="2">
         <v>1</v>
       </c>
@@ -1194,8 +1267,9 @@
         <v>66</v>
       </c>
       <c r="F48" s="4"/>
-    </row>
-    <row r="49" spans="2:6" ht="101.25" customHeight="1">
+      <c r="G48" s="18"/>
+    </row>
+    <row r="49" spans="2:7" ht="101.25" customHeight="1">
       <c r="C49" s="2">
         <v>2</v>
       </c>
@@ -1207,7 +1281,7 @@
       </c>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="2:6" ht="105.75" customHeight="1">
+    <row r="50" spans="2:7" ht="105.75" customHeight="1">
       <c r="C50" s="2">
         <v>3</v>
       </c>
@@ -1219,7 +1293,7 @@
       </c>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="2:6" ht="80.25" customHeight="1">
+    <row r="51" spans="2:7" ht="80.25" customHeight="1">
       <c r="C51" s="2">
         <v>4</v>
       </c>
@@ -1231,7 +1305,7 @@
       </c>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="2:6" ht="88.5" customHeight="1">
+    <row r="52" spans="2:7" ht="88.5" customHeight="1">
       <c r="C52" s="2">
         <v>5</v>
       </c>
@@ -1243,7 +1317,7 @@
       </c>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="2:6" ht="90.75" customHeight="1">
+    <row r="53" spans="2:7" ht="90.75" customHeight="1">
       <c r="C53" s="2">
         <v>6</v>
       </c>
@@ -1255,7 +1329,7 @@
       </c>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="2:6" ht="24" customHeight="1">
+    <row r="54" spans="2:7" ht="24" customHeight="1">
       <c r="C54" s="15" t="s">
         <v>54</v>
       </c>
@@ -1263,7 +1337,7 @@
       <c r="E54" s="15"/>
       <c r="F54" s="15"/>
     </row>
-    <row r="55" spans="2:6" ht="24" customHeight="1">
+    <row r="55" spans="2:7" ht="24" customHeight="1">
       <c r="B55" s="6"/>
       <c r="C55" s="9" t="s">
         <v>55</v>
@@ -1271,8 +1345,11 @@
       <c r="D55" s="10"/>
       <c r="E55" s="10"/>
       <c r="F55" s="11"/>
-    </row>
-    <row r="56" spans="2:6" ht="102.75" customHeight="1">
+      <c r="G55" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="102.75" customHeight="1">
       <c r="C56" s="2">
         <v>1</v>
       </c>
@@ -1284,7 +1361,7 @@
       </c>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="2:6" ht="69" customHeight="1">
+    <row r="57" spans="2:7" ht="69" customHeight="1">
       <c r="C57" s="2">
         <v>2</v>
       </c>
@@ -1296,7 +1373,7 @@
       </c>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="2:6" ht="93.75" customHeight="1">
+    <row r="58" spans="2:7" ht="93.75" customHeight="1">
       <c r="C58" s="2">
         <v>3</v>
       </c>
@@ -1308,7 +1385,7 @@
       </c>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="2:6" ht="78.75" customHeight="1">
+    <row r="59" spans="2:7" ht="78.75" customHeight="1">
       <c r="C59" s="2">
         <v>4</v>
       </c>
@@ -1320,15 +1397,18 @@
       </c>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="2:6" ht="25.5" customHeight="1">
+    <row r="60" spans="2:7" ht="25.5" customHeight="1">
       <c r="C60" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
       <c r="F60" s="11"/>
-    </row>
-    <row r="61" spans="2:6" ht="67.5" customHeight="1">
+      <c r="G60" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="67.5" customHeight="1">
       <c r="C61" s="2">
         <v>1</v>
       </c>
@@ -1339,8 +1419,9 @@
         <v>64</v>
       </c>
       <c r="F61" s="4"/>
-    </row>
-    <row r="62" spans="2:6" ht="84" customHeight="1">
+      <c r="G61" s="18"/>
+    </row>
+    <row r="62" spans="2:7" ht="84" customHeight="1">
       <c r="C62" s="2">
         <v>2</v>
       </c>
@@ -1352,7 +1433,7 @@
       </c>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="2:6" ht="84.75" customHeight="1">
+    <row r="63" spans="2:7" ht="84.75" customHeight="1">
       <c r="C63" s="2">
         <v>3</v>
       </c>
@@ -1364,15 +1445,18 @@
       </c>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="2:6" s="6" customFormat="1" ht="34.15" customHeight="1">
+    <row r="64" spans="2:7" s="6" customFormat="1" ht="34.200000000000003" customHeight="1">
       <c r="C64" s="9" t="s">
         <v>77</v>
       </c>
       <c r="D64" s="10"/>
       <c r="E64" s="10"/>
       <c r="F64" s="11"/>
-    </row>
-    <row r="65" spans="3:6" ht="38.25">
+      <c r="G64" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7" ht="39.6">
       <c r="C65" s="2">
         <v>1</v>
       </c>
@@ -1383,8 +1467,9 @@
         <v>64</v>
       </c>
       <c r="F65" s="4"/>
-    </row>
-    <row r="66" spans="3:6" ht="76.5">
+      <c r="G65" s="18"/>
+    </row>
+    <row r="66" spans="3:7" ht="79.2">
       <c r="C66" s="2">
         <v>2</v>
       </c>
@@ -1396,7 +1481,7 @@
       </c>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" spans="3:6" ht="51">
+    <row r="67" spans="3:7" ht="52.8">
       <c r="C67" s="2">
         <v>3</v>
       </c>
@@ -1408,7 +1493,7 @@
       </c>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" spans="3:6" ht="51">
+    <row r="68" spans="3:7" ht="52.8">
       <c r="C68" s="2">
         <v>4</v>
       </c>
@@ -1420,7 +1505,7 @@
       </c>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="3:6" ht="51">
+    <row r="69" spans="3:7" ht="52.8">
       <c r="C69" s="2">
         <v>5</v>
       </c>
@@ -1432,7 +1517,7 @@
       </c>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" spans="3:6" ht="63.75">
+    <row r="70" spans="3:7" ht="66">
       <c r="C70" s="2">
         <v>6</v>
       </c>
@@ -1445,7 +1530,13 @@
       <c r="F70" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="14">
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G60:G61"/>
     <mergeCell ref="C55:F55"/>
     <mergeCell ref="C60:F60"/>
     <mergeCell ref="C64:F64"/>
@@ -1456,6 +1547,6 @@
     <mergeCell ref="C54:F54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51181102362204689" footer="0.51181102362204689"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>